<commit_message>
this is the second
</commit_message>
<xml_diff>
--- a/src/test/resources/inputData/Data.xlsx
+++ b/src/test/resources/inputData/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shaiq\eclipse-workspace\com.tekschool.hotel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baria\git\UpdateDataDrivenFramework\src\test\resources\inputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3710FDC-8397-45B9-AF73-F19C33A79703}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0618789-3D41-46D8-951C-FE00DEE26CA7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>firstName</t>
   </si>
@@ -67,6 +67,15 @@
   </si>
   <si>
     <t>user@test.com</t>
+  </si>
+  <si>
+    <t>baryalai</t>
+  </si>
+  <si>
+    <t>joyan</t>
+  </si>
+  <si>
+    <t>user2</t>
   </si>
 </sst>
 </file>
@@ -395,21 +404,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.3984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -423,7 +432,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -437,7 +446,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -451,7 +460,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -463,6 +472,20 @@
       </c>
       <c r="D4" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -470,6 +493,7 @@
     <hyperlink ref="C2" r:id="rId1" xr:uid="{AEC963B9-504D-4F67-924C-5EAE91E94728}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{C99EAF03-7C9A-4534-A110-CF482A579FC9}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{429AA696-7376-4302-810E-C1499B96939F}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{FBFBACB1-A58F-4CB0-A4E4-5F2081A78307}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>